<commit_message>
include pars excel and load db
</commit_message>
<xml_diff>
--- a/List_Microsoft_Excel_2.xlsx
+++ b/List_Microsoft_Excel_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moder\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vsevolod\Documents\AppHakaton1\AppHakaton1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C22909-B933-4DCE-8320-461C3784CFA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7D9866-FCF4-4FA0-883E-8C90B12854BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,34 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
-  <si>
-    <t>Дата рейса</t>
-  </si>
-  <si>
-    <t>Время по расписанию</t>
-  </si>
-  <si>
-    <t>Код авиакомпании</t>
-  </si>
-  <si>
-    <t>Номер рейса</t>
-  </si>
-  <si>
-    <t>Флаг прилет/вылет</t>
-  </si>
-  <si>
-    <t>Тип ВС</t>
-  </si>
-  <si>
-    <t>Стоянка ВС</t>
-  </si>
-  <si>
-    <t>Стоянка сектор</t>
-  </si>
-  <si>
-    <t>Название авиакомпании</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>N4</t>
   </si>
@@ -97,18 +70,6 @@
   </si>
   <si>
     <t>32A</t>
-  </si>
-  <si>
-    <t>SU9</t>
-  </si>
-  <si>
-    <t>109W</t>
-  </si>
-  <si>
-    <t>Терминал B</t>
-  </si>
-  <si>
-    <t>32B</t>
   </si>
 </sst>
 </file>
@@ -428,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,32 +408,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1">
+        <v>43951</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1">
+        <v>721</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1">
+        <v>772</v>
+      </c>
+      <c r="G1">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -480,28 +441,28 @@
         <v>43951</v>
       </c>
       <c r="B2" s="2">
-        <v>0.87152777777777779</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>721</v>
+        <v>1130</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>772</v>
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>59</v>
+        <v>162</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -509,28 +470,28 @@
         <v>43951</v>
       </c>
       <c r="B3" s="2">
-        <v>0.95833333333333337</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1130</v>
+        <v>279</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>162</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -538,28 +499,28 @@
         <v>43951</v>
       </c>
       <c r="B4" s="2">
-        <v>0.97222222222222221</v>
+        <v>0.97569444444444453</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>185</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="D4">
-        <v>279</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
         <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -567,28 +528,28 @@
         <v>43951</v>
       </c>
       <c r="B5" s="2">
-        <v>0.97569444444444453</v>
+        <v>0.78472222222222221</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>185</v>
+        <v>273</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -596,144 +557,28 @@
         <v>43951</v>
       </c>
       <c r="B6" s="2">
-        <v>0.78472222222222221</v>
+        <v>0.98611111111111116</v>
       </c>
       <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1863</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>273</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
       <c r="I6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>43951</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.98611111111111116</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>1863</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7">
-        <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>43951</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.98958333333333337</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>113</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>43951</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.98958333333333337</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>43951</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.99652777777777779</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10">
-        <v>1956</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10">
-        <v>31</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>